<commit_message>
revisions of Sarka's annotation of parentless nodes
</commit_message>
<xml_diff>
--- a/data/annotations/cs/2020_04_complete_morphseg/annotated/completeseg-1100-ZZ.xlsx
+++ b/data/annotations/cs/2020_04_complete_morphseg/annotated/completeseg-1100-ZZ.xlsx
@@ -6277,7 +6277,7 @@
     <t xml:space="preserve">jankovský</t>
   </si>
   <si>
-    <t xml:space="preserve">jankov sk ý</t>
+    <t xml:space="preserve">jan k ov sk ý</t>
   </si>
   <si>
     <t xml:space="preserve">reklama</t>
@@ -6473,8 +6473,8 @@
   </sheetPr>
   <dimension ref="A1:F1101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1066" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1102" activeCellId="0" sqref="E1102"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A622" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E640" activeCellId="0" sqref="E640"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>